<commit_message>
Added up to date example data
</commit_message>
<xml_diff>
--- a/example_data/FarmToFork_GENERATOR_Contacts.xlsx
+++ b/example_data/FarmToFork_GENERATOR_Contacts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fraser/code/ftf/example_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasbrierley/Desktop/Work/GFO/Test_Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E3D974-E4A5-9440-8351-D9E66673683D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969B05D2-5EAB-374D-9557-E6EEE6CDA26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{8F378BB0-B83A-A44D-8EFE-3CC700C1BBAE}"/>
   </bookViews>
@@ -167,9 +167,6 @@
     <t>62 Woodstock Rd</t>
   </si>
   <si>
-    <t>Manor Rd</t>
-  </si>
-  <si>
     <t>Queen's Ln</t>
   </si>
   <si>
@@ -269,26 +266,29 @@
     <t>Lady Margaret Hall</t>
   </si>
   <si>
+    <t>St Antony's College</t>
+  </si>
+  <si>
+    <t>Exeter</t>
+  </si>
+  <si>
+    <t>Exeter College</t>
+  </si>
+  <si>
+    <t>OX1 3DP</t>
+  </si>
+  <si>
     <t>St Antony's</t>
   </si>
   <si>
-    <t>St Antony's College</t>
-  </si>
-  <si>
-    <t>Exeter</t>
-  </si>
-  <si>
-    <t>Exeter College</t>
-  </si>
-  <si>
-    <t>OX1 3DP</t>
+    <t xml:space="preserve">Manor Rd </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -308,6 +308,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -330,10 +336,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66AE39D3-A9D3-124B-A0F9-8AE5C0919E49}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,10 +676,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>12</v>
@@ -681,13 +688,13 @@
         <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="H1" s="2"/>
     </row>
@@ -696,7 +703,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -736,10 +743,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
@@ -753,324 +760,327 @@
     </row>
     <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>78</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:16" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="P28" t="s">
-        <v>58</v>
+        <v>31</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P29" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>